<commit_message>
Updating repo with Dashboard code
</commit_message>
<xml_diff>
--- a/CalorieTracker.xlsx
+++ b/CalorieTracker.xlsx
@@ -400,7 +400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -530,6 +530,43 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07/07/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3 eggs omlette</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>561</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added input.html for Text Input prompt
</commit_message>
<xml_diff>
--- a/CalorieTracker.xlsx
+++ b/CalorieTracker.xlsx
@@ -400,7 +400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -641,6 +641,314 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1 bun butter</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1 bun butter</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1 bun butter</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1 bun butter</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1 protein pudding worth 25 gm protein</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1 protein pudding worth 25 gm protein</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1 protein pudding worth 25 gm protein</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1 bana smoothie with greek yoghurt</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>15/07/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1 bana smoothie with greek yoghurt</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>